<commit_message>
2000 for some, plus Campo Grande
</commit_message>
<xml_diff>
--- a/VIDA2/data/FORTALEZA.xlsx
+++ b/VIDA2/data/FORTALEZA.xlsx
@@ -465,13 +465,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8.639278557114228</v>
+        <v>8.493</v>
       </c>
       <c r="D2" t="n">
-        <v>139.1444503019819</v>
+        <v>138.2121050110019</v>
       </c>
       <c r="E2" t="n">
-        <v>50.16308739017312</v>
+        <v>49.62052522640749</v>
       </c>
     </row>
     <row r="3">
@@ -484,13 +484,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>13.294</v>
+        <v>13.076</v>
       </c>
       <c r="D3" t="n">
-        <v>123.4098919592694</v>
+        <v>133.724422794741</v>
       </c>
       <c r="E3" t="n">
-        <v>43.58816647711178</v>
+        <v>45.34742009920699</v>
       </c>
     </row>
     <row r="4">
@@ -503,13 +503,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>16.32</v>
+        <v>16.3745</v>
       </c>
       <c r="D4" t="n">
-        <v>134.1865452910149</v>
+        <v>134.4024185004127</v>
       </c>
       <c r="E4" t="n">
-        <v>49.12558429201854</v>
+        <v>46.80138294083683</v>
       </c>
     </row>
     <row r="5">
@@ -522,13 +522,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10.208</v>
+        <v>10.194</v>
       </c>
       <c r="D5" t="n">
-        <v>127.8875538805879</v>
+        <v>124.8242952223214</v>
       </c>
       <c r="E5" t="n">
-        <v>47.93300648439967</v>
+        <v>43.15758203999295</v>
       </c>
     </row>
     <row r="6">
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12.706</v>
+        <v>12.686</v>
       </c>
       <c r="D6" t="n">
-        <v>124.0631698427504</v>
+        <v>119.3313039155821</v>
       </c>
       <c r="E6" t="n">
-        <v>42.36268755884785</v>
+        <v>42.27009763250305</v>
       </c>
     </row>
     <row r="7">
@@ -560,13 +560,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10.61</v>
+        <v>10.6605</v>
       </c>
       <c r="D7" t="n">
-        <v>115.0768775256391</v>
+        <v>129.9043036426934</v>
       </c>
       <c r="E7" t="n">
-        <v>47.28926865188473</v>
+        <v>46.96046931654505</v>
       </c>
     </row>
     <row r="8">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11.818</v>
+        <v>11.8485</v>
       </c>
       <c r="D8" t="n">
-        <v>121.2450040499577</v>
+        <v>130.2577837810884</v>
       </c>
       <c r="E8" t="n">
-        <v>43.33299137223285</v>
+        <v>47.44206003759771</v>
       </c>
     </row>
     <row r="9">
@@ -598,13 +598,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>12.308</v>
+        <v>12.649</v>
       </c>
       <c r="D9" t="n">
-        <v>135.5014940795732</v>
+        <v>133.1804077043862</v>
       </c>
       <c r="E9" t="n">
-        <v>46.61295318589364</v>
+        <v>50.42680369922832</v>
       </c>
     </row>
     <row r="10">
@@ -617,13 +617,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>11.734</v>
+        <v>11.48</v>
       </c>
       <c r="D10" t="n">
-        <v>120.4311211148672</v>
+        <v>122.0408321174531</v>
       </c>
       <c r="E10" t="n">
-        <v>39.7337789489492</v>
+        <v>43.45788686073116</v>
       </c>
     </row>
     <row r="11">
@@ -636,13 +636,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8.308617234468938</v>
+        <v>8.479739869934967</v>
       </c>
       <c r="D11" t="n">
-        <v>124.8096383425866</v>
+        <v>113.1072278773255</v>
       </c>
       <c r="E11" t="n">
-        <v>39.7259172972364</v>
+        <v>39.32327553762875</v>
       </c>
     </row>
     <row r="12">
@@ -655,13 +655,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>11.002</v>
+        <v>10.993</v>
       </c>
       <c r="D12" t="n">
-        <v>128.3865013125848</v>
+        <v>124.4132729899284</v>
       </c>
       <c r="E12" t="n">
-        <v>45.43893140742988</v>
+        <v>44.45632428352587</v>
       </c>
     </row>
     <row r="13">
@@ -674,13 +674,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>16.038</v>
+        <v>16.037</v>
       </c>
       <c r="D13" t="n">
-        <v>122.4069866922088</v>
+        <v>123.4990470279122</v>
       </c>
       <c r="E13" t="n">
-        <v>45.49748352949253</v>
+        <v>44.54230880144893</v>
       </c>
     </row>
     <row r="14">
@@ -693,13 +693,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>15.738</v>
+        <v>15.567</v>
       </c>
       <c r="D14" t="n">
-        <v>120.1873799992845</v>
+        <v>124.8102756395077</v>
       </c>
       <c r="E14" t="n">
-        <v>43.05388905075726</v>
+        <v>45.17456018663325</v>
       </c>
     </row>
     <row r="15">
@@ -712,13 +712,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>13.012</v>
+        <v>13.092</v>
       </c>
       <c r="D15" t="n">
-        <v>123.1435683474182</v>
+        <v>122.3369515471478</v>
       </c>
       <c r="E15" t="n">
-        <v>45.99501810501608</v>
+        <v>43.04066583061345</v>
       </c>
     </row>
     <row r="16">
@@ -731,13 +731,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>11.086</v>
+        <v>10.8895</v>
       </c>
       <c r="D16" t="n">
-        <v>112.2639929729713</v>
+        <v>114.133759584069</v>
       </c>
       <c r="E16" t="n">
-        <v>40.11226358780539</v>
+        <v>41.11978358328968</v>
       </c>
     </row>
     <row r="17">
@@ -750,13 +750,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>20.85</v>
+        <v>20.7745</v>
       </c>
       <c r="D17" t="n">
-        <v>121.4316744157692</v>
+        <v>119.7904317012385</v>
       </c>
       <c r="E17" t="n">
-        <v>42.37851356971846</v>
+        <v>43.67321504267104</v>
       </c>
     </row>
     <row r="18">
@@ -769,13 +769,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>11.024</v>
+        <v>11.2105</v>
       </c>
       <c r="D18" t="n">
-        <v>124.4556606362332</v>
+        <v>123.9404751314064</v>
       </c>
       <c r="E18" t="n">
-        <v>41.94254389401446</v>
+        <v>44.9234908680257</v>
       </c>
     </row>
     <row r="19">
@@ -788,13 +788,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>12.048</v>
+        <v>12.3865</v>
       </c>
       <c r="D19" t="n">
-        <v>129.1350783844712</v>
+        <v>126.0523788868359</v>
       </c>
       <c r="E19" t="n">
-        <v>48.66041701683846</v>
+        <v>45.24503448563813</v>
       </c>
     </row>
     <row r="20">
@@ -807,13 +807,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>12.166</v>
+        <v>12.366</v>
       </c>
       <c r="D20" t="n">
-        <v>122.3193035808361</v>
+        <v>124.1930982632989</v>
       </c>
       <c r="E20" t="n">
-        <v>45.42207015550667</v>
+        <v>45.76236901851799</v>
       </c>
     </row>
     <row r="21">
@@ -826,13 +826,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>26.51</v>
+        <v>26.1105</v>
       </c>
       <c r="D21" t="n">
-        <v>111.4226287805192</v>
+        <v>112.9804929442418</v>
       </c>
       <c r="E21" t="n">
-        <v>38.98579591033202</v>
+        <v>39.19356157752623</v>
       </c>
     </row>
     <row r="22">
@@ -845,13 +845,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>40.606</v>
+        <v>40.4025</v>
       </c>
       <c r="D22" t="n">
-        <v>123.8819181466714</v>
+        <v>124.3732943371092</v>
       </c>
       <c r="E22" t="n">
-        <v>45.05486246169889</v>
+        <v>44.36426455680216</v>
       </c>
     </row>
     <row r="23">
@@ -864,13 +864,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>30.858</v>
+        <v>30.6325</v>
       </c>
       <c r="D23" t="n">
-        <v>123.7242385525245</v>
+        <v>129.284449854257</v>
       </c>
       <c r="E23" t="n">
-        <v>42.7816428905438</v>
+        <v>46.50544765803853</v>
       </c>
     </row>
     <row r="24">
@@ -883,13 +883,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>20.718</v>
+        <v>20.689</v>
       </c>
       <c r="D24" t="n">
-        <v>127.933503203073</v>
+        <v>126.6597244057631</v>
       </c>
       <c r="E24" t="n">
-        <v>46.21160706028198</v>
+        <v>46.27972834875423</v>
       </c>
     </row>
     <row r="25">
@@ -902,13 +902,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>27.746</v>
+        <v>28.045</v>
       </c>
       <c r="D25" t="n">
-        <v>124.4050085171968</v>
+        <v>120.1315782805712</v>
       </c>
       <c r="E25" t="n">
-        <v>42.55922867267152</v>
+        <v>43.31127238957166</v>
       </c>
     </row>
     <row r="26">
@@ -921,13 +921,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>24.802</v>
+        <v>25.0135</v>
       </c>
       <c r="D26" t="n">
-        <v>127.2347863535552</v>
+        <v>127.7096151952027</v>
       </c>
       <c r="E26" t="n">
-        <v>48.09571261872103</v>
+        <v>45.8962232724554</v>
       </c>
     </row>
     <row r="27">
@@ -940,13 +940,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>19.416</v>
+        <v>19.5465</v>
       </c>
       <c r="D27" t="n">
-        <v>123.3514464642694</v>
+        <v>117.6965821438448</v>
       </c>
       <c r="E27" t="n">
-        <v>45.12176898732314</v>
+        <v>40.91965001322355</v>
       </c>
     </row>
     <row r="28">
@@ -959,13 +959,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>29.716</v>
+        <v>29.499</v>
       </c>
       <c r="D28" t="n">
-        <v>128.0693524289109</v>
+        <v>126.1577462205547</v>
       </c>
       <c r="E28" t="n">
-        <v>44.04548276700515</v>
+        <v>45.96968192093264</v>
       </c>
     </row>
     <row r="29">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>23.04</v>
+        <v>23.124</v>
       </c>
       <c r="D29" t="n">
-        <v>120.6517446878505</v>
+        <v>123.2868255339318</v>
       </c>
       <c r="E29" t="n">
-        <v>41.82701030386552</v>
+        <v>43.84169611219947</v>
       </c>
     </row>
     <row r="30">
@@ -997,13 +997,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>19.944</v>
+        <v>19.67</v>
       </c>
       <c r="D30" t="n">
-        <v>120.2823183552585</v>
+        <v>120.614835547111</v>
       </c>
       <c r="E30" t="n">
-        <v>40.65912584414394</v>
+        <v>44.45851403096109</v>
       </c>
     </row>
     <row r="31">
@@ -1016,13 +1016,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>23.83</v>
+        <v>24.0245</v>
       </c>
       <c r="D31" t="n">
-        <v>116.3768981635882</v>
+        <v>117.932922579168</v>
       </c>
       <c r="E31" t="n">
-        <v>43.89361842395827</v>
+        <v>43.89835938733413</v>
       </c>
     </row>
     <row r="32">
@@ -1035,13 +1035,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>22.516</v>
+        <v>22.4185</v>
       </c>
       <c r="D32" t="n">
-        <v>122.2334180929721</v>
+        <v>111.86193452914</v>
       </c>
       <c r="E32" t="n">
-        <v>47.08570029099851</v>
+        <v>40.76446116482944</v>
       </c>
     </row>
     <row r="33">
@@ -1054,13 +1054,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>25.34</v>
+        <v>25.3905</v>
       </c>
       <c r="D33" t="n">
-        <v>120.836188056846</v>
+        <v>123.0227978889059</v>
       </c>
       <c r="E33" t="n">
-        <v>41.9797971986523</v>
+        <v>44.67464632822779</v>
       </c>
     </row>
     <row r="34">
@@ -1073,13 +1073,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>19.644</v>
+        <v>19.8615</v>
       </c>
       <c r="D34" t="n">
-        <v>131.8327549871765</v>
+        <v>126.5022610162921</v>
       </c>
       <c r="E34" t="n">
-        <v>50.28109080403384</v>
+        <v>45.83943887983695</v>
       </c>
     </row>
     <row r="35">
@@ -1092,13 +1092,13 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>26.196</v>
+        <v>26.605</v>
       </c>
       <c r="D35" t="n">
-        <v>122.2219232188007</v>
+        <v>119.9188253966303</v>
       </c>
       <c r="E35" t="n">
-        <v>42.35600713336316</v>
+        <v>43.40972418172567</v>
       </c>
     </row>
     <row r="36">
@@ -1111,13 +1111,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>23.402</v>
+        <v>23.4655</v>
       </c>
       <c r="D36" t="n">
-        <v>118.2268266288413</v>
+        <v>118.6185173210186</v>
       </c>
       <c r="E36" t="n">
-        <v>38.77287442904295</v>
+        <v>43.86352969802942</v>
       </c>
     </row>
     <row r="37">
@@ -1130,13 +1130,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>16.45</v>
+        <v>16.464</v>
       </c>
       <c r="D37" t="n">
-        <v>123.1996173644834</v>
+        <v>128.4666661445988</v>
       </c>
       <c r="E37" t="n">
-        <v>46.36832845629116</v>
+        <v>44.70570920892852</v>
       </c>
     </row>
     <row r="38">
@@ -1149,13 +1149,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>37.546</v>
+        <v>37.9305</v>
       </c>
       <c r="D38" t="n">
-        <v>130.652851695118</v>
+        <v>130.6428033553322</v>
       </c>
       <c r="E38" t="n">
-        <v>43.81466968252957</v>
+        <v>46.96319501419122</v>
       </c>
     </row>
     <row r="39">
@@ -1168,13 +1168,13 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>43.146</v>
+        <v>43.119</v>
       </c>
       <c r="D39" t="n">
-        <v>123.0593956226941</v>
+        <v>124.7641549377724</v>
       </c>
       <c r="E39" t="n">
-        <v>42.25999263643832</v>
+        <v>44.46416927360076</v>
       </c>
     </row>
     <row r="40">
@@ -1187,13 +1187,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>22.382</v>
+        <v>22.2865</v>
       </c>
       <c r="D40" t="n">
-        <v>130.6732744055899</v>
+        <v>122.1016069333414</v>
       </c>
       <c r="E40" t="n">
-        <v>44.98223954780497</v>
+        <v>45.64695081092949</v>
       </c>
     </row>
     <row r="41">
@@ -1206,13 +1206,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>19.234</v>
+        <v>19.123</v>
       </c>
       <c r="D41" t="n">
-        <v>121.3672448398151</v>
+        <v>123.1994271847872</v>
       </c>
       <c r="E41" t="n">
-        <v>42.86905326386188</v>
+        <v>45.14760521342026</v>
       </c>
     </row>
     <row r="42">
@@ -1225,13 +1225,13 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>33.06</v>
+        <v>33.386</v>
       </c>
       <c r="D42" t="n">
-        <v>121.1167721016228</v>
+        <v>125.7933177743727</v>
       </c>
       <c r="E42" t="n">
-        <v>45.16039911205023</v>
+        <v>45.41316105069031</v>
       </c>
     </row>
     <row r="43">
@@ -1244,13 +1244,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>26.054</v>
+        <v>25.753</v>
       </c>
       <c r="D43" t="n">
-        <v>121.8741816575865</v>
+        <v>123.4384839462759</v>
       </c>
       <c r="E43" t="n">
-        <v>46.9166507195317</v>
+        <v>44.89023328146816</v>
       </c>
     </row>
     <row r="44">
@@ -1263,13 +1263,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>26.262</v>
+        <v>26.5235</v>
       </c>
       <c r="D44" t="n">
-        <v>122.3674283557411</v>
+        <v>122.6782950557239</v>
       </c>
       <c r="E44" t="n">
-        <v>43.60513611914868</v>
+        <v>43.46841679227594</v>
       </c>
     </row>
     <row r="45">
@@ -1282,13 +1282,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>17.256</v>
+        <v>17.3625</v>
       </c>
       <c r="D45" t="n">
-        <v>124.8049503494922</v>
+        <v>125.7777356093641</v>
       </c>
       <c r="E45" t="n">
-        <v>40.64839662513979</v>
+        <v>44.9576992291684</v>
       </c>
     </row>
     <row r="46">
@@ -1301,13 +1301,13 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>26.792</v>
+        <v>26.245</v>
       </c>
       <c r="D46" t="n">
-        <v>126.984006151527</v>
+        <v>124.8381548245996</v>
       </c>
       <c r="E46" t="n">
-        <v>44.99606333378859</v>
+        <v>44.83715592540979</v>
       </c>
     </row>
     <row r="47">
@@ -1320,13 +1320,13 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>29.684</v>
+        <v>29.768</v>
       </c>
       <c r="D47" t="n">
-        <v>120.892403264841</v>
+        <v>119.6360391913562</v>
       </c>
       <c r="E47" t="n">
-        <v>43.74640557786947</v>
+        <v>42.8661141550626</v>
       </c>
     </row>
     <row r="48">
@@ -1339,13 +1339,13 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>18.972</v>
+        <v>18.7615</v>
       </c>
       <c r="D48" t="n">
-        <v>119.3524606968738</v>
+        <v>117.7217521278933</v>
       </c>
       <c r="E48" t="n">
-        <v>41.81367400690922</v>
+        <v>42.48942735894942</v>
       </c>
     </row>
     <row r="49">
@@ -1358,13 +1358,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>27.844</v>
+        <v>27.1565</v>
       </c>
       <c r="D49" t="n">
-        <v>118.4417984718428</v>
+        <v>121.2788130664943</v>
       </c>
       <c r="E49" t="n">
-        <v>41.76066772269585</v>
+        <v>42.9537963788505</v>
       </c>
     </row>
     <row r="50">
@@ -1377,13 +1377,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>27.916</v>
+        <v>27.6375</v>
       </c>
       <c r="D50" t="n">
-        <v>120.9046923048323</v>
+        <v>124.3998904561981</v>
       </c>
       <c r="E50" t="n">
-        <v>42.9998558087871</v>
+        <v>44.42896293157964</v>
       </c>
     </row>
     <row r="51">
@@ -1396,13 +1396,13 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>24.586</v>
+        <v>24.7065</v>
       </c>
       <c r="D51" t="n">
-        <v>128.8890312987808</v>
+        <v>124.2234291629387</v>
       </c>
       <c r="E51" t="n">
-        <v>46.05084341258824</v>
+        <v>44.42912191241763</v>
       </c>
     </row>
     <row r="52">
@@ -1415,13 +1415,13 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>30.624</v>
+        <v>30.5025</v>
       </c>
       <c r="D52" t="n">
-        <v>120.9193156630717</v>
+        <v>122.1040240562442</v>
       </c>
       <c r="E52" t="n">
-        <v>44.34451717359558</v>
+        <v>43.66704522659213</v>
       </c>
     </row>
     <row r="53">
@@ -1434,13 +1434,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>24.19</v>
+        <v>24.024</v>
       </c>
       <c r="D53" t="n">
-        <v>121.5823351374541</v>
+        <v>127.2968482125203</v>
       </c>
       <c r="E53" t="n">
-        <v>43.1450952105894</v>
+        <v>44.76188997770294</v>
       </c>
     </row>
     <row r="54">
@@ -1453,13 +1453,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>21.11</v>
+        <v>21.0075</v>
       </c>
       <c r="D54" t="n">
-        <v>131.0298761365121</v>
+        <v>124.2570040038955</v>
       </c>
       <c r="E54" t="n">
-        <v>45.95903706310551</v>
+        <v>45.93153660877089</v>
       </c>
     </row>
     <row r="55">
@@ -1472,13 +1472,13 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>23.542</v>
+        <v>23.328</v>
       </c>
       <c r="D55" t="n">
-        <v>124.8935205655266</v>
+        <v>121.5165721498364</v>
       </c>
       <c r="E55" t="n">
-        <v>46.6512758469791</v>
+        <v>43.44747212895968</v>
       </c>
     </row>
     <row r="56">
@@ -1491,13 +1491,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>28.76</v>
+        <v>28.3465</v>
       </c>
       <c r="D56" t="n">
-        <v>120.6678139029936</v>
+        <v>125.0621436325535</v>
       </c>
       <c r="E56" t="n">
-        <v>43.24761860600707</v>
+        <v>45.52099802126362</v>
       </c>
     </row>
     <row r="57">
@@ -1510,13 +1510,13 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>19.402</v>
+        <v>20.0295</v>
       </c>
       <c r="D57" t="n">
-        <v>125.2791450992594</v>
+        <v>123.5175162519351</v>
       </c>
       <c r="E57" t="n">
-        <v>45.39103672964474</v>
+        <v>43.96558039626111</v>
       </c>
     </row>
     <row r="58">
@@ -1529,13 +1529,13 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>29.19</v>
+        <v>29.047</v>
       </c>
       <c r="D58" t="n">
-        <v>127.0599481083362</v>
+        <v>120.6837828087753</v>
       </c>
       <c r="E58" t="n">
-        <v>45.89657430638366</v>
+        <v>43.43892656750148</v>
       </c>
     </row>
     <row r="59">
@@ -1548,13 +1548,13 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>35.41</v>
+        <v>35.516</v>
       </c>
       <c r="D59" t="n">
-        <v>125.3258324843328</v>
+        <v>125.906498143847</v>
       </c>
       <c r="E59" t="n">
-        <v>45.39473128928243</v>
+        <v>45.1850784580714</v>
       </c>
     </row>
     <row r="60">
@@ -1567,13 +1567,13 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>27.32</v>
+        <v>27.433</v>
       </c>
       <c r="D60" t="n">
-        <v>130.5564067825154</v>
+        <v>120.6160884633927</v>
       </c>
       <c r="E60" t="n">
-        <v>44.21512645376576</v>
+        <v>42.49924264697203</v>
       </c>
     </row>
     <row r="61">
@@ -1586,13 +1586,13 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>42.684</v>
+        <v>42.2105</v>
       </c>
       <c r="D61" t="n">
-        <v>121.3321481449327</v>
+        <v>120.8558399094228</v>
       </c>
       <c r="E61" t="n">
-        <v>42.60097631796244</v>
+        <v>44.43362372145269</v>
       </c>
     </row>
     <row r="62">
@@ -1605,13 +1605,13 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>23.964</v>
+        <v>23.7505</v>
       </c>
       <c r="D62" t="n">
-        <v>127.2553984341011</v>
+        <v>126.5800968572592</v>
       </c>
       <c r="E62" t="n">
-        <v>43.69160456001942</v>
+        <v>43.33915063635087</v>
       </c>
     </row>
     <row r="63">
@@ -1624,13 +1624,13 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>28.688</v>
+        <v>28.077</v>
       </c>
       <c r="D63" t="n">
-        <v>115.9762781783708</v>
+        <v>122.1727064227149</v>
       </c>
       <c r="E63" t="n">
-        <v>41.28203891762261</v>
+        <v>43.18891017195162</v>
       </c>
     </row>
     <row r="64">
@@ -1643,13 +1643,13 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>18.956</v>
+        <v>19.3365</v>
       </c>
       <c r="D64" t="n">
-        <v>115.5372922778439</v>
+        <v>121.3143484870903</v>
       </c>
       <c r="E64" t="n">
-        <v>41.10161488080443</v>
+        <v>45.59630086374899</v>
       </c>
     </row>
     <row r="65">
@@ -1662,13 +1662,13 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>18.466</v>
+        <v>18.423</v>
       </c>
       <c r="D65" t="n">
-        <v>116.295293002353</v>
+        <v>120.8662923674692</v>
       </c>
       <c r="E65" t="n">
-        <v>38.70124906493757</v>
+        <v>42.51264322627399</v>
       </c>
     </row>
     <row r="66">
@@ -1681,13 +1681,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>17.778</v>
+        <v>17.764</v>
       </c>
       <c r="D66" t="n">
-        <v>126.6756983283736</v>
+        <v>127.9054229939492</v>
       </c>
       <c r="E66" t="n">
-        <v>47.56745437631477</v>
+        <v>46.43035465408656</v>
       </c>
     </row>
     <row r="67">
@@ -1700,13 +1700,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>19.648</v>
+        <v>20.2435</v>
       </c>
       <c r="D67" t="n">
-        <v>131.6137956031421</v>
+        <v>126.1563009237087</v>
       </c>
       <c r="E67" t="n">
-        <v>47.39381600339973</v>
+        <v>44.31421487530822</v>
       </c>
     </row>
     <row r="68">
@@ -1719,13 +1719,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>17.546</v>
+        <v>17.5785</v>
       </c>
       <c r="D68" t="n">
-        <v>119.5083199559364</v>
+        <v>124.5868299400943</v>
       </c>
       <c r="E68" t="n">
-        <v>42.20501142439439</v>
+        <v>45.51216446328593</v>
       </c>
     </row>
     <row r="69">
@@ -1738,13 +1738,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>22.672</v>
+        <v>22.8485</v>
       </c>
       <c r="D69" t="n">
-        <v>129.9449872174707</v>
+        <v>123.3242793770075</v>
       </c>
       <c r="E69" t="n">
-        <v>45.51043481442954</v>
+        <v>42.99361142299753</v>
       </c>
     </row>
     <row r="70">
@@ -1757,13 +1757,13 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>29.566</v>
+        <v>29.647</v>
       </c>
       <c r="D70" t="n">
-        <v>131.6449289346992</v>
+        <v>126.9010605471866</v>
       </c>
       <c r="E70" t="n">
-        <v>46.6160804010936</v>
+        <v>45.35747458615094</v>
       </c>
     </row>
     <row r="71">
@@ -1776,13 +1776,13 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>24.16</v>
+        <v>23.683</v>
       </c>
       <c r="D71" t="n">
-        <v>130.9251699141939</v>
+        <v>124.5155703400955</v>
       </c>
       <c r="E71" t="n">
-        <v>45.36738470421356</v>
+        <v>44.93812250754635</v>
       </c>
     </row>
     <row r="72">
@@ -1795,13 +1795,13 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>28.566</v>
+        <v>28.9135</v>
       </c>
       <c r="D72" t="n">
-        <v>132.1865808170687</v>
+        <v>125.7831669278456</v>
       </c>
       <c r="E72" t="n">
-        <v>47.49823098959278</v>
+        <v>44.19720923779696</v>
       </c>
     </row>
     <row r="73">
@@ -1814,13 +1814,13 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>21.1</v>
+        <v>21.051</v>
       </c>
       <c r="D73" t="n">
-        <v>128.3002898041717</v>
+        <v>125.2565901081983</v>
       </c>
       <c r="E73" t="n">
-        <v>42.42714951917759</v>
+        <v>45.65880044087243</v>
       </c>
     </row>
     <row r="74">
@@ -1833,13 +1833,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>21.37</v>
+        <v>21.5235</v>
       </c>
       <c r="D74" t="n">
-        <v>120.0130326022212</v>
+        <v>123.1405194308701</v>
       </c>
       <c r="E74" t="n">
-        <v>41.39384398112617</v>
+        <v>44.4610649907541</v>
       </c>
     </row>
     <row r="75">
@@ -1852,13 +1852,13 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>20.706</v>
+        <v>20.45</v>
       </c>
       <c r="D75" t="n">
-        <v>126.3102182732885</v>
+        <v>128.0800927780364</v>
       </c>
       <c r="E75" t="n">
-        <v>46.34369953167992</v>
+        <v>46.51488790619788</v>
       </c>
     </row>
     <row r="76">
@@ -1871,13 +1871,13 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>7.3687374749499</v>
+        <v>7.3005</v>
       </c>
       <c r="D76" t="n">
-        <v>139.882015374176</v>
+        <v>138.9903022115482</v>
       </c>
       <c r="E76" t="n">
-        <v>46.63474468083685</v>
+        <v>49.35503637444425</v>
       </c>
     </row>
     <row r="77">
@@ -1890,13 +1890,13 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>10.634</v>
+        <v>10.8375</v>
       </c>
       <c r="D77" t="n">
-        <v>126.7020165936574</v>
+        <v>132.0461306516838</v>
       </c>
       <c r="E77" t="n">
-        <v>45.51328434207692</v>
+        <v>45.34729557078619</v>
       </c>
     </row>
     <row r="78">
@@ -1909,13 +1909,13 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>11.138</v>
+        <v>11.039</v>
       </c>
       <c r="D78" t="n">
-        <v>118.5235402712182</v>
+        <v>126.6721430258688</v>
       </c>
       <c r="E78" t="n">
-        <v>40.67935780250018</v>
+        <v>43.90391794952542</v>
       </c>
     </row>
     <row r="79">
@@ -1928,13 +1928,13 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>8.390000000000001</v>
+        <v>8.648824412206103</v>
       </c>
       <c r="D79" t="n">
-        <v>121.3479908979908</v>
+        <v>122.5541177536137</v>
       </c>
       <c r="E79" t="n">
-        <v>45.67706460206458</v>
+        <v>43.00702832431927</v>
       </c>
     </row>
     <row r="80">
@@ -1947,13 +1947,13 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>8.190380761523047</v>
+        <v>8.092000000000001</v>
       </c>
       <c r="D80" t="n">
-        <v>124.4448779180005</v>
+        <v>129.1117256002509</v>
       </c>
       <c r="E80" t="n">
-        <v>40.51156481016199</v>
+        <v>44.81449778721446</v>
       </c>
     </row>
     <row r="81">
@@ -1966,13 +1966,13 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>11.028</v>
+        <v>10.85</v>
       </c>
       <c r="D81" t="n">
-        <v>121.026372878927</v>
+        <v>124.8396526813396</v>
       </c>
       <c r="E81" t="n">
-        <v>42.59545494924752</v>
+        <v>43.91739014339618</v>
       </c>
     </row>
     <row r="82">
@@ -1985,13 +1985,13 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>10.786</v>
+        <v>10.98</v>
       </c>
       <c r="D82" t="n">
-        <v>121.9620598682363</v>
+        <v>119.9599367110354</v>
       </c>
       <c r="E82" t="n">
-        <v>46.27638825227061</v>
+        <v>42.25896625819989</v>
       </c>
     </row>
     <row r="83">
@@ -2004,13 +2004,13 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>7.68</v>
+        <v>7.744372186093046</v>
       </c>
       <c r="D83" t="n">
-        <v>135.1140775890776</v>
+        <v>124.0549642430728</v>
       </c>
       <c r="E83" t="n">
-        <v>46.86236263736262</v>
+        <v>42.98942669966414</v>
       </c>
     </row>
     <row r="84">
@@ -2023,13 +2023,13 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>9.390000000000001</v>
+        <v>9.438499999999999</v>
       </c>
       <c r="D84" t="n">
-        <v>131.1866227253997</v>
+        <v>124.7367657432863</v>
       </c>
       <c r="E84" t="n">
-        <v>49.7011791699872</v>
+        <v>47.42504873437529</v>
       </c>
     </row>
     <row r="85">
@@ -2042,13 +2042,13 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>12.982</v>
+        <v>13.371</v>
       </c>
       <c r="D85" t="n">
-        <v>130.4310521081049</v>
+        <v>121.3136445451626</v>
       </c>
       <c r="E85" t="n">
-        <v>48.54702878521694</v>
+        <v>44.48955015622463</v>
       </c>
     </row>
     <row r="86">
@@ -2061,13 +2061,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>9.404</v>
+        <v>9.025</v>
       </c>
       <c r="D86" t="n">
-        <v>122.2824339059632</v>
+        <v>131.7103658274125</v>
       </c>
       <c r="E86" t="n">
-        <v>44.61847482582776</v>
+        <v>46.70712937947839</v>
       </c>
     </row>
     <row r="87">
@@ -2080,13 +2080,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>10.826</v>
+        <v>10.967</v>
       </c>
       <c r="D87" t="n">
-        <v>125.4732158965904</v>
+        <v>126.0323425478026</v>
       </c>
       <c r="E87" t="n">
-        <v>44.22394422742713</v>
+        <v>45.99226633789319</v>
       </c>
     </row>
     <row r="88">
@@ -2099,13 +2099,13 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>12.63</v>
+        <v>12.6075</v>
       </c>
       <c r="D88" t="n">
-        <v>124.8497936617906</v>
+        <v>119.571531103952</v>
       </c>
       <c r="E88" t="n">
-        <v>43.92707432746133</v>
+        <v>43.21443715835317</v>
       </c>
     </row>
     <row r="89">
@@ -2118,13 +2118,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>9.036</v>
+        <v>9.198</v>
       </c>
       <c r="D89" t="n">
-        <v>126.8943556357642</v>
+        <v>131.1268325671573</v>
       </c>
       <c r="E89" t="n">
-        <v>43.46241576620829</v>
+        <v>52.14753511237635</v>
       </c>
     </row>
     <row r="90">
@@ -2137,13 +2137,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>9.311999999999999</v>
+        <v>9.3835</v>
       </c>
       <c r="D90" t="n">
-        <v>121.160636748872</v>
+        <v>121.7874297851268</v>
       </c>
       <c r="E90" t="n">
-        <v>45.51534152122383</v>
+        <v>43.3335133197555</v>
       </c>
     </row>
     <row r="91">
@@ -2156,13 +2156,13 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>10.478</v>
+        <v>10.268</v>
       </c>
       <c r="D91" t="n">
-        <v>124.7558143610774</v>
+        <v>130.3277896488612</v>
       </c>
       <c r="E91" t="n">
-        <v>45.93092911560399</v>
+        <v>44.73702373692692</v>
       </c>
     </row>
     <row r="92">
@@ -2175,13 +2175,13 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>15.318</v>
+        <v>15.4485</v>
       </c>
       <c r="D92" t="n">
-        <v>125.8073145144292</v>
+        <v>126.0345079486912</v>
       </c>
       <c r="E92" t="n">
-        <v>42.11864315512786</v>
+        <v>44.72208461430241</v>
       </c>
     </row>
     <row r="93">
@@ -2194,13 +2194,13 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>16.556</v>
+        <v>16.559</v>
       </c>
       <c r="D93" t="n">
-        <v>128.7506770518186</v>
+        <v>127.6228491322402</v>
       </c>
       <c r="E93" t="n">
-        <v>44.17668142673795</v>
+        <v>47.06405964797976</v>
       </c>
     </row>
     <row r="94">
@@ -2213,13 +2213,13 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>8.970000000000001</v>
+        <v>9.086499999999999</v>
       </c>
       <c r="D94" t="n">
-        <v>124.7757123509445</v>
+        <v>122.1223049417902</v>
       </c>
       <c r="E94" t="n">
-        <v>46.67527072171034</v>
+        <v>44.43852095616796</v>
       </c>
     </row>
     <row r="95">
@@ -2232,13 +2232,13 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>13.162</v>
+        <v>12.998</v>
       </c>
       <c r="D95" t="n">
-        <v>120.0640319291693</v>
+        <v>123.3109748395488</v>
       </c>
       <c r="E95" t="n">
-        <v>42.55936245041509</v>
+        <v>43.60772706944863</v>
       </c>
     </row>
     <row r="96">
@@ -2251,13 +2251,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>17.188</v>
+        <v>17.344</v>
       </c>
       <c r="D96" t="n">
-        <v>119.5423134994894</v>
+        <v>121.2718692900091</v>
       </c>
       <c r="E96" t="n">
-        <v>47.59867043326332</v>
+        <v>43.46750151385268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>